<commit_message>
Add fitting code for diffusion coefficients. Modify totalCrank to accept matrices. Add file for fitting. Add datasheet for fitting data. fitting
</commit_message>
<xml_diff>
--- a/CranksModelInfo.xlsx
+++ b/CranksModelInfo.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ecfile1.uwaterloo.ca\atreid\My Documents\4B\temp\FYDP-master\FYDP-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ecfile1.uwaterloo.ca\atreid\My Documents\4B\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="10">
   <si>
     <t>Particle Radius</t>
   </si>
@@ -392,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,7 +467,7 @@
         <v>0.7</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F11" si="0">1-E3</f>
+        <f t="shared" ref="F3:F8" si="0">1-E3</f>
         <v>0.30000000000000004</v>
       </c>
       <c r="G3">
@@ -581,20 +581,24 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>13</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>0.42</v>
+        <f>B9/$B$9</f>
+        <v>1</v>
       </c>
       <c r="F9">
-        <f t="shared" si="0"/>
-        <v>0.58000000000000007</v>
+        <f>1-E9</f>
+        <v>0</v>
       </c>
       <c r="G9">
         <v>200</v>
@@ -602,20 +606,24 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>9.4</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>73</v>
+        <v>8</v>
       </c>
       <c r="E10">
-        <v>0.37</v>
+        <f>B10/$B$9</f>
+        <v>0.72307692307692306</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
-        <v>0.63</v>
+        <f t="shared" ref="F10:F12" si="1">1-E10</f>
+        <v>0.27692307692307694</v>
       </c>
       <c r="G10">
         <v>200</v>
@@ -623,20 +631,24 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="E11">
-        <v>0.36</v>
+        <f>B11/$B$9</f>
+        <v>0.61538461538461542</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
-        <v>0.64</v>
+        <f t="shared" si="1"/>
+        <v>0.38461538461538458</v>
       </c>
       <c r="G11">
         <v>200</v>
@@ -647,21 +659,21 @@
         <v>6</v>
       </c>
       <c r="B12">
-        <v>13</v>
+        <v>7.3</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="E12">
-        <f t="shared" ref="E12:E16" si="1">B12/$B$12</f>
-        <v>1</v>
+        <f>B12/$B$9</f>
+        <v>0.56153846153846154</v>
       </c>
       <c r="F12">
-        <f>1-E12</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.43846153846153846</v>
       </c>
       <c r="G12">
         <v>200</v>
@@ -669,24 +681,24 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B13">
-        <v>9.4</v>
+        <v>0.7</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D13">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <f t="shared" si="1"/>
-        <v>0.72307692307692306</v>
+        <f t="shared" ref="E13:E21" si="2">B13/$B$13</f>
+        <v>1</v>
       </c>
       <c r="F13">
-        <f t="shared" ref="F13:F16" si="2">1-E13</f>
-        <v>0.27692307692307694</v>
+        <f>1-E13</f>
+        <v>0</v>
       </c>
       <c r="G13">
         <v>200</v>
@@ -694,24 +706,24 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B14">
-        <v>8</v>
+        <v>0.45</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="E14">
-        <f t="shared" si="1"/>
-        <v>0.61538461538461542</v>
+        <f t="shared" si="2"/>
+        <v>0.6428571428571429</v>
       </c>
       <c r="F14">
-        <f t="shared" si="2"/>
-        <v>0.38461538461538458</v>
+        <f t="shared" ref="F14:F21" si="3">1-E14</f>
+        <v>0.3571428571428571</v>
       </c>
       <c r="G14">
         <v>200</v>
@@ -719,24 +731,24 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B15">
-        <v>7.3</v>
+        <v>0.52</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D15">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="E15">
-        <f t="shared" si="1"/>
-        <v>0.56153846153846154</v>
+        <f t="shared" si="2"/>
+        <v>0.74285714285714288</v>
       </c>
       <c r="F15">
-        <f t="shared" si="2"/>
-        <v>0.43846153846153846</v>
+        <f t="shared" si="3"/>
+        <v>0.25714285714285712</v>
       </c>
       <c r="G15">
         <v>200</v>
@@ -744,24 +756,24 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B16">
-        <v>7.2</v>
+        <v>0.43</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D16">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="E16">
-        <f t="shared" si="1"/>
-        <v>0.55384615384615388</v>
+        <f t="shared" si="2"/>
+        <v>0.61428571428571432</v>
       </c>
       <c r="F16">
-        <f t="shared" si="2"/>
-        <v>0.44615384615384612</v>
+        <f t="shared" si="3"/>
+        <v>0.38571428571428568</v>
       </c>
       <c r="G16">
         <v>200</v>
@@ -772,21 +784,21 @@
         <v>7</v>
       </c>
       <c r="B17">
-        <v>0.7</v>
+        <v>0.42</v>
       </c>
       <c r="C17">
         <v>3</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E17">
-        <f t="shared" ref="E17:E25" si="3">B17/$B$17</f>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>0.6</v>
       </c>
       <c r="F17">
-        <f>1-E17</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.4</v>
       </c>
       <c r="G17">
         <v>200</v>
@@ -797,21 +809,21 @@
         <v>7</v>
       </c>
       <c r="B18">
-        <v>0.45</v>
+        <v>0.41</v>
       </c>
       <c r="C18">
         <v>3</v>
       </c>
       <c r="D18">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E18">
+        <f t="shared" si="2"/>
+        <v>0.58571428571428574</v>
+      </c>
+      <c r="F18">
         <f t="shared" si="3"/>
-        <v>0.6428571428571429</v>
-      </c>
-      <c r="F18">
-        <f t="shared" ref="F18:F25" si="4">1-E18</f>
-        <v>0.3571428571428571</v>
+        <v>0.41428571428571426</v>
       </c>
       <c r="G18">
         <v>200</v>
@@ -822,21 +834,21 @@
         <v>7</v>
       </c>
       <c r="B19">
-        <v>0.52</v>
+        <v>0.39</v>
       </c>
       <c r="C19">
         <v>3</v>
       </c>
       <c r="D19">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="E19">
+        <f t="shared" si="2"/>
+        <v>0.55714285714285716</v>
+      </c>
+      <c r="F19">
         <f t="shared" si="3"/>
-        <v>0.74285714285714288</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="4"/>
-        <v>0.25714285714285712</v>
+        <v>0.44285714285714284</v>
       </c>
       <c r="G19">
         <v>200</v>
@@ -847,21 +859,21 @@
         <v>7</v>
       </c>
       <c r="B20">
-        <v>0.43</v>
+        <v>0.36</v>
       </c>
       <c r="C20">
         <v>3</v>
       </c>
       <c r="D20">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="E20">
+        <f t="shared" si="2"/>
+        <v>0.51428571428571435</v>
+      </c>
+      <c r="F20">
         <f t="shared" si="3"/>
-        <v>0.61428571428571432</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="4"/>
-        <v>0.38571428571428568</v>
+        <v>0.48571428571428565</v>
       </c>
       <c r="G20">
         <v>200</v>
@@ -872,123 +884,23 @@
         <v>7</v>
       </c>
       <c r="B21">
-        <v>0.42</v>
+        <v>0.34</v>
       </c>
       <c r="C21">
         <v>3</v>
       </c>
       <c r="D21">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="E21">
+        <f t="shared" si="2"/>
+        <v>0.48571428571428577</v>
+      </c>
+      <c r="F21">
         <f t="shared" si="3"/>
-        <v>0.6</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="4"/>
-        <v>0.4</v>
+        <v>0.51428571428571423</v>
       </c>
       <c r="G21">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22">
-        <v>0.41</v>
-      </c>
-      <c r="C22">
-        <v>3</v>
-      </c>
-      <c r="D22">
-        <v>16</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="3"/>
-        <v>0.58571428571428574</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="4"/>
-        <v>0.41428571428571426</v>
-      </c>
-      <c r="G22">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23">
-        <v>0.39</v>
-      </c>
-      <c r="C23">
-        <v>3</v>
-      </c>
-      <c r="D23">
-        <v>24</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="3"/>
-        <v>0.55714285714285716</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="4"/>
-        <v>0.44285714285714284</v>
-      </c>
-      <c r="G23">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24">
-        <v>0.36</v>
-      </c>
-      <c r="C24">
-        <v>3</v>
-      </c>
-      <c r="D24">
-        <v>28</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="3"/>
-        <v>0.51428571428571435</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="4"/>
-        <v>0.48571428571428565</v>
-      </c>
-      <c r="G24">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25">
-        <v>0.34</v>
-      </c>
-      <c r="C25">
-        <v>3</v>
-      </c>
-      <c r="D25">
-        <v>40</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="3"/>
-        <v>0.48571428571428577</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="4"/>
-        <v>0.51428571428571423</v>
-      </c>
-      <c r="G25">
         <v>200</v>
       </c>
     </row>

</xml_diff>